<commit_message>
Added more test data from excel file
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestDataShareSkill.xlsx
+++ b/MarsFramework/ExcelData/TestDataShareSkill.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\MVPStudio-MarsProject\Internship-Mars\Assignments\Assignment-2\PageFactory\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0110D5E6-97E5-4B95-BAC0-A1A2F25ADDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F91EF2-C818-4CC7-B568-7341F4A7D48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,13 +17,14 @@
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
     <sheet name="ShareSkill" sheetId="2" r:id="rId3"/>
     <sheet name="DeleteSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="EditSkill" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Url</t>
   </si>
@@ -149,6 +150,54 @@
   </si>
   <si>
     <t>Automation</t>
+  </si>
+  <si>
+    <t>EditedCreditAmount</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Programming Language</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>AddingData</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t>SQL Queries</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Markup Language</t>
+  </si>
+  <si>
+    <t>Web &amp; Mobile App</t>
+  </si>
+  <si>
+    <t>Webpage Design</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>8:00AM</t>
+  </si>
+  <si>
+    <t>Web Design</t>
   </si>
 </sst>
 </file>
@@ -656,16 +705,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="20.15234375" customWidth="1"/>
-    <col min="4" max="4" width="15.07421875" customWidth="1"/>
+    <col min="1" max="1" width="20.15234375" customWidth="1"/>
+    <col min="2" max="2" width="25.61328125" customWidth="1"/>
+    <col min="3" max="3" width="20.15234375" customWidth="1"/>
+    <col min="4" max="4" width="23.3046875" customWidth="1"/>
     <col min="5" max="5" width="18.3046875" customWidth="1"/>
     <col min="6" max="6" width="24.84375" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
@@ -782,6 +833,112 @@
         <v>5</v>
       </c>
       <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="3">
+        <v>44638</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44638</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="3">
+        <v>44641</v>
+      </c>
+      <c r="I4" s="3">
+        <v>44641</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -824,4 +981,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BE3ACA-AFD7-4A45-AA1D-3CDE067906F3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.23046875" customWidth="1"/>
+    <col min="2" max="2" width="17.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>